<commit_message>
update cloud related figures
</commit_message>
<xml_diff>
--- a/analysis/stat.xlsx
+++ b/analysis/stat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au686295_uni_au_dk/Documents/Documents/GitHub/PhD/orbit-drift-MODIS-ice-albedo/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au686295\GitHub\PhD\orbit-drift-MODIS-ice-albedo\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{50D04801-8064-4591-A851-1DFBA94ABECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEE1FB56-0E26-4D51-90E1-7175E51E3DA1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208C774D-6864-4814-A94D-74EFBED2CAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="2160" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{49D7E878-2DD4-473C-8D14-502A01B15A7E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{49D7E878-2DD4-473C-8D14-502A01B15A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="dt" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="HSA" sheetId="3" r:id="rId3"/>
     <sheet name="S3" sheetId="5" r:id="rId4"/>
     <sheet name="MYD" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>MYD(2002-2019)</t>
   </si>
@@ -94,9 +95,6 @@
     <t>2002-2019</t>
   </si>
   <si>
-    <t>MYD</t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
   <si>
@@ -104,6 +102,54 @@
   </si>
   <si>
     <t>2002-2018</t>
+  </si>
+  <si>
+    <t>MYD10</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>kpc_l</t>
+  </si>
+  <si>
+    <t>nuk_k</t>
+  </si>
+  <si>
+    <t>nuk_l</t>
+  </si>
+  <si>
+    <t>qas_l</t>
+  </si>
+  <si>
+    <t>qas_m</t>
+  </si>
+  <si>
+    <t>qas_u</t>
+  </si>
+  <si>
+    <t>tas_l</t>
+  </si>
+  <si>
+    <t>thu_l</t>
+  </si>
+  <si>
+    <t>thu_u</t>
+  </si>
+  <si>
+    <t>thu_u2</t>
+  </si>
+  <si>
+    <t>upe_u</t>
+  </si>
+  <si>
+    <t>upe_l</t>
+  </si>
+  <si>
+    <t>egp</t>
+  </si>
+  <si>
+    <t>kan_l</t>
   </si>
 </sst>
 </file>
@@ -3126,10 +3172,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3430,7 +3472,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3542,7 +3584,7 @@
         <v>0.01</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7">
         <f>B8-dt!E7</f>
@@ -3557,7 +3599,7 @@
         <v>1.35E-2</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="8">
         <v>1.2999999999999999E-2</v>
@@ -3571,7 +3613,7 @@
         <v>1.35E-2</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8">
         <v>5.0999999999999995E-3</v>
@@ -3585,7 +3627,7 @@
         <v>1.35E-2</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="8">
         <v>8.8000000000000005E-3</v>
@@ -3764,7 +3806,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="9">
         <f>MEDIAN(B4:B20)</f>
@@ -3990,13 +4032,13 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4089,7 +4131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4041A7E-6E72-46F8-925A-BDA46EA8ACDA}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -4263,4 +4305,241 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4403F7B-3062-4325-B14C-23063D9A07F0}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="8">
+        <v>-0.17</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-0.23</v>
+      </c>
+      <c r="D2" s="8">
+        <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.48</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.88</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.43</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.92</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="8">
+        <v>-0.09</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.67</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.31</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.65</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>